<commit_message>
Programa finalizado, a pulir
</commit_message>
<xml_diff>
--- a/Checklist Equipos RRHH.xlsx
+++ b/Checklist Equipos RRHH.xlsx
@@ -615,7 +615,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -712,8 +712,16 @@
           <t>TV Planta baja</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr"/>
-      <c r="C4" s="21" t="inlineStr"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C4" s="21" t="inlineStr">
+        <is>
+          <t>que</t>
+        </is>
+      </c>
       <c r="D4" s="18" t="n"/>
       <c r="F4" t="inlineStr">
         <is>
@@ -737,8 +745,16 @@
           <t>TV Primer Piso</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr"/>
-      <c r="C5" s="21" t="inlineStr"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>sb</t>
+        </is>
+      </c>
+      <c r="C5" s="21" t="inlineStr">
+        <is>
+          <t>sdb</t>
+        </is>
+      </c>
       <c r="D5" s="18" t="n"/>
     </row>
     <row r="6" ht="16.5" customHeight="1" s="16">
@@ -747,8 +763,16 @@
           <t>Totem PB</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr"/>
-      <c r="C6" s="21" t="inlineStr"/>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>3434</t>
+        </is>
+      </c>
+      <c r="C6" s="21" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
       <c r="D6" s="18" t="n"/>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
optimized the code, deleted some lines and edited the code to not use an external .py to work with the excel file
</commit_message>
<xml_diff>
--- a/Checklist Equipos RRHH.xlsx
+++ b/Checklist Equipos RRHH.xlsx
@@ -618,7 +618,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col width="15.140625" bestFit="1" customWidth="1" style="16" min="1" max="1"/>
     <col width="25.42578125" bestFit="1" customWidth="1" style="16" min="2" max="2"/>
@@ -712,7 +712,11 @@
           <t>TV Planta baja</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>dsd</t>
+        </is>
+      </c>
       <c r="C4" s="21" t="inlineStr"/>
       <c r="D4" s="18" t="n"/>
       <c r="F4" t="inlineStr">
@@ -737,7 +741,11 @@
           <t>TV Primer Piso</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>bfb</t>
+        </is>
+      </c>
       <c r="C5" s="21" t="inlineStr"/>
       <c r="D5" s="18" t="n"/>
     </row>
@@ -747,8 +755,16 @@
           <t>Totem PB</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr"/>
-      <c r="C6" s="21" t="inlineStr"/>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="C6" s="21" t="inlineStr">
+        <is>
+          <t>1r1</t>
+        </is>
+      </c>
       <c r="D6" s="18" t="n"/>
     </row>
     <row r="7">
@@ -819,7 +835,7 @@
       </c>
       <c r="B17" s="19" t="inlineStr">
         <is>
-          <t>1123123</t>
+          <t>ewfwegwgewg</t>
         </is>
       </c>
       <c r="C17" s="20" t="n"/>

</xml_diff>

<commit_message>
Se modificaron las funciones
</commit_message>
<xml_diff>
--- a/Checklist Equipos RRHH.xlsx
+++ b/Checklist Equipos RRHH.xlsx
@@ -714,7 +714,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>dsd</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="C4" s="21" t="inlineStr"/>
@@ -743,10 +743,14 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>bfb</t>
-        </is>
-      </c>
-      <c r="C5" s="21" t="inlineStr"/>
+          <t>apagada</t>
+        </is>
+      </c>
+      <c r="C5" s="21" t="inlineStr">
+        <is>
+          <t>encendida</t>
+        </is>
+      </c>
       <c r="D5" s="18" t="n"/>
     </row>
     <row r="6" ht="16.5" customHeight="1" s="16">
@@ -757,12 +761,12 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>444</t>
+          <t>apagado</t>
         </is>
       </c>
       <c r="C6" s="21" t="inlineStr">
         <is>
-          <t>1r1</t>
+          <t>monitor roto</t>
         </is>
       </c>
       <c r="D6" s="18" t="n"/>
@@ -835,7 +839,7 @@
       </c>
       <c r="B17" s="19" t="inlineStr">
         <is>
-          <t>ewfwegwgewg</t>
+          <t>d12d1212d12d</t>
         </is>
       </c>
       <c r="C17" s="20" t="n"/>

</xml_diff>